<commit_message>
Added Java Program for Telegram Bot
</commit_message>
<xml_diff>
--- a/Pandas/TelegramBot/ekyc_data.xlsx
+++ b/Pandas/TelegramBot/ekyc_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Agent Login</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>weekly</t>
   </si>
 </sst>
 </file>
@@ -373,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,44 +396,59 @@
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>110</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>23</v>
       </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>35</v>
       </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>123</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>